<commit_message>
Automatic Backpropogation using _backward() function
</commit_message>
<xml_diff>
--- a/AndrejKarpathyZero-HeroProgressTracker.xlsx
+++ b/AndrejKarpathyZero-HeroProgressTracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junai\Desktop\DataScienceClasses\Andrej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A14A40F-5F68-4C01-95C5-D664FE8D9613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE33B47-7384-493B-9FA5-EDF5395F3B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{172AED4A-7BA1-42C3-A446-FCB562FCC5B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ANDREJ KARPATHY LLM COURSE</t>
   </si>
@@ -60,6 +61,24 @@
   </si>
   <si>
     <t>Manual Backpropogation, grad</t>
+  </si>
+  <si>
+    <t>Andrej Karpathy</t>
+  </si>
+  <si>
+    <t>Langchain</t>
+  </si>
+  <si>
+    <t>5 day AI Agents</t>
+  </si>
+  <si>
+    <t>Illustrated DSA Book</t>
+  </si>
+  <si>
+    <t>75 blind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic Backpropogation through _backward, tanh </t>
   </si>
 </sst>
 </file>
@@ -448,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC55F3-4978-4FD1-B3AF-8D7E266867B7}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +534,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
@@ -523,4 +550,47 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D02C4B-3445-4E09-B9F9-DF530C479AC9}">
+  <dimension ref="C5:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added Neuron, Layer functionality. PyTorch Implemetation
</commit_message>
<xml_diff>
--- a/AndrejKarpathyZero-HeroProgressTracker.xlsx
+++ b/AndrejKarpathyZero-HeroProgressTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junai\Desktop\DataScienceClasses\Andrej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE33B47-7384-493B-9FA5-EDF5395F3B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D978A0-507C-42CD-9DDB-73F0F4E487F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{172AED4A-7BA1-42C3-A446-FCB562FCC5B5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ANDREJ KARPATHY LLM COURSE</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t xml:space="preserve">Automatic Backpropogation through _backward, tanh </t>
+  </si>
+  <si>
+    <t>Implemented exp, pow, div, sub, Neuron, Layers</t>
   </si>
 </sst>
 </file>
@@ -122,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,6 +135,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC55F3-4978-4FD1-B3AF-8D7E266867B7}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,8 +544,16 @@
       <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>